<commit_message>
Update sample codes using MinUnit test framework.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/min_unit_sample_data.xlsx
+++ b/doc/sample/test_sample_input/min_unit_sample_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="テスト一覧" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="106">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -570,6 +570,18 @@
   </si>
   <si>
     <t>subFuncA_002_subInput1[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>_input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>input2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;_input2[0]</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -687,7 +699,37 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <border>
+        <top/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <border>
+        <top/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <border>
+        <top/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1116,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1988,12 +2030,12 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:P21">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>M10=M9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3224,17 +3266,17 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D8 M12:P27 M29:P30 M32:P32">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:P28">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>M28=M27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:P31">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>M31=M29</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3245,9 +3287,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AC27"/>
+  <dimension ref="B2:AC28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16:AC16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3264,9 +3308,9 @@
     <col min="12" max="12" width="2.375" style="5" customWidth="1"/>
     <col min="13" max="13" width="9.625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="45" width="3" style="5" customWidth="1"/>
     <col min="46" max="16384" width="2.125" style="5"/>
   </cols>
@@ -3616,7 +3660,7 @@
         <v>3</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="6">
@@ -3674,26 +3718,48 @@
         <v>3</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B17" s="8"/>
@@ -3710,32 +3776,24 @@
         <v>3</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Q17" s="6">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-      <c r="X17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
     </row>
@@ -3754,33 +3812,33 @@
         <v>3</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="6">
-        <v>2</v>
-      </c>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="U18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V18" s="3"/>
       <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="X18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="AA18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.15">
@@ -3798,34 +3856,34 @@
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>42</v>
       </c>
       <c r="Q19" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3" t="s">
+      <c r="S19" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3" t="s">
+      <c r="V19" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Y19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="AB19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC19" s="3"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B20" s="8"/>
@@ -3836,30 +3894,40 @@
       <c r="G20" s="9"/>
       <c r="H20" s="8"/>
       <c r="M20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Q20" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="T20" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
+      <c r="W20" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="Z20" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
+      <c r="AC20" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B21" s="8"/>
@@ -3880,29 +3948,17 @@
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="6">
-        <v>1</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
       <c r="U21" s="3"/>
-      <c r="V21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="W21" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
@@ -3926,32 +3982,32 @@
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="6">
-        <v>2</v>
-      </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC22" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B23" s="8"/>
@@ -3972,20 +4028,32 @@
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="X23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
+      <c r="AA23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC23" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B24" s="8"/>
@@ -3999,33 +4067,27 @@
         <v>36</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
-      <c r="AC24" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="AC24" s="3"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B25" s="8"/>
@@ -4046,30 +4108,26 @@
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="6">
-        <v>10</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3" t="s">
+      <c r="U25" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="V25" s="3"/>
       <c r="W25" s="3"/>
-      <c r="X25" s="3" t="s">
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
-      <c r="AB25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B26" s="8"/>
@@ -4090,25 +4148,29 @@
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="6">
-        <v>20</v>
-      </c>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3" t="s">
+      <c r="V26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="X26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3" t="s">
+      <c r="Z26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AC26" s="3"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.15">
@@ -4123,48 +4185,61 @@
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
+      <c r="W27" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="3"/>
+      <c r="AA27" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
     </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.15">
+      <c r="M28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="6">
+        <v>30</v>
+      </c>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C4:D7 M21:P23 M11:P15 M17:O19">
-    <cfRule type="expression" dxfId="6" priority="4">
+  <conditionalFormatting sqref="C4:E7 M11:P28">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>C4=C3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M24:P27">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>M24=M23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M20:P20">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>M20=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16:O16">
-    <cfRule type="expression" dxfId="3" priority="8">
-      <formula>M16=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P16:P19">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>P16=P15</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4795,12 +4870,12 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D10">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:P25">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>M14=M13</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update sample input data.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/min_unit_sample_data.xlsx
+++ b/doc/sample/test_sample_input/min_unit_sample_data.xlsx
@@ -11,14 +11,13 @@
     <sheet name="sample_function_001" sheetId="1" r:id="rId2"/>
     <sheet name="sample_function_002" sheetId="3" r:id="rId3"/>
     <sheet name="sample_function_003" sheetId="4" r:id="rId4"/>
-    <sheet name="sample_function_004" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="97">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -189,10 +188,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>subFuncA</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>subInput1</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -300,48 +295,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>グローバル変数</t>
-    <rPh sb="5" eb="7">
-      <t>ヘンスウ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>内部</t>
-    <rPh sb="0" eb="2">
-      <t>ナイブ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>外部</t>
-    <rPh sb="0" eb="2">
-      <t>ガイブ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>*</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>**</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>short</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>long</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>insideVariable</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>outsideVariable</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -699,97 +653,7 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <border>
-        <top/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1172,7 +1036,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1200,13 +1064,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -1214,13 +1078,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -1228,13 +1092,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -1285,19 +1149,19 @@
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -1326,7 +1190,7 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.15">
@@ -1345,7 +1209,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J5" s="6"/>
     </row>
@@ -1365,27 +1229,27 @@
         <v>25</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J6" s="6"/>
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.15">
       <c r="L8" s="10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:33" x14ac:dyDescent="0.15">
       <c r="M9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="Q9" s="4" t="s">
         <v>2</v>
@@ -1441,7 +1305,7 @@
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.15">
       <c r="M10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>3</v>
@@ -1450,22 +1314,22 @@
         <v>9</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="6">
         <v>0</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
@@ -1489,7 +1353,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="M11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>3</v>
@@ -1498,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q11" s="6">
         <v>1</v>
@@ -1508,16 +1372,16 @@
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
@@ -1537,7 +1401,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="8"/>
       <c r="M12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>3</v>
@@ -1546,7 +1410,7 @@
         <v>9</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q12" s="6">
         <v>2</v>
@@ -1560,16 +1424,16 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
@@ -1585,7 +1449,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="M13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>3</v>
@@ -1594,7 +1458,7 @@
         <v>9</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q13" s="6">
         <v>3</v>
@@ -1612,16 +1476,16 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AF13" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.15">
@@ -1633,7 +1497,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="M14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>3</v>
@@ -1642,31 +1506,31 @@
         <v>10</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="6">
         <v>0</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
@@ -1681,7 +1545,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="M15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>3</v>
@@ -1690,32 +1554,32 @@
         <v>11</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q15" s="6">
         <v>1</v>
       </c>
       <c r="R15" s="3"/>
       <c r="S15" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
@@ -1729,7 +1593,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="M16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>3</v>
@@ -1738,7 +1602,7 @@
         <v>11</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q16" s="6">
         <v>2</v>
@@ -1746,25 +1610,25 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AG16" s="3"/>
     </row>
@@ -1777,7 +1641,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="M17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>3</v>
@@ -1786,7 +1650,7 @@
         <v>11</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q17" s="6">
         <v>3</v>
@@ -1795,25 +1659,25 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
       <c r="AG17" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.15">
@@ -1825,41 +1689,41 @@
       <c r="G18" s="9"/>
       <c r="H18" s="8"/>
       <c r="M18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="6">
         <v>0</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.15">
@@ -1871,13 +1735,13 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="M19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="6">
@@ -1885,30 +1749,30 @@
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
       <c r="AF19" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="AG19" s="3"/>
     </row>
@@ -1921,13 +1785,13 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="M20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="6">
@@ -1936,24 +1800,24 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
       <c r="AE20" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
@@ -1967,13 +1831,13 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="M21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="6">
@@ -1983,7 +1847,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
@@ -1994,7 +1858,7 @@
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
@@ -2030,12 +1894,12 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D6">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:P21">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>M10=M9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2079,19 +1943,19 @@
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -2116,11 +1980,11 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.15">
@@ -2176,7 +2040,7 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -2194,7 +2058,7 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>26</v>
@@ -2203,21 +2067,21 @@
     </row>
     <row r="10" spans="2:33" x14ac:dyDescent="0.15">
       <c r="L10" s="10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.15">
       <c r="M11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>2</v>
@@ -2273,7 +2137,7 @@
     </row>
     <row r="12" spans="2:33" x14ac:dyDescent="0.15">
       <c r="M12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>3</v>
@@ -2282,7 +2146,7 @@
         <v>9</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -2297,7 +2161,7 @@
         <v>12</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
@@ -2321,7 +2185,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="M13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>3</v>
@@ -2330,7 +2194,7 @@
         <v>9</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q13" s="6">
         <v>1</v>
@@ -2340,16 +2204,16 @@
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X13" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
@@ -2369,7 +2233,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="8"/>
       <c r="M14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>3</v>
@@ -2378,7 +2242,7 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q14" s="6">
         <v>2</v>
@@ -2392,16 +2256,16 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="AD14" s="3"/>
       <c r="AE14" s="3"/>
@@ -2417,7 +2281,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="M15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>3</v>
@@ -2426,7 +2290,7 @@
         <v>9</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q15" s="6">
         <v>3</v>
@@ -2444,16 +2308,16 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AF15" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AG15" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.15">
@@ -2465,7 +2329,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="M16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>3</v>
@@ -2474,31 +2338,31 @@
         <v>10</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q16" s="6">
         <v>0</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
@@ -2513,7 +2377,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="M17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>3</v>
@@ -2522,7 +2386,7 @@
         <v>10</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q17" s="6">
         <v>1</v>
@@ -2561,7 +2425,7 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="M18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>3</v>
@@ -2570,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q18" s="6">
         <v>2</v>
@@ -2609,7 +2473,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="M19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>3</v>
@@ -2618,7 +2482,7 @@
         <v>10</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q19" s="6">
         <v>3</v>
@@ -2627,25 +2491,25 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AD19" s="3"/>
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.15">
@@ -2657,38 +2521,38 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="M20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="6">
         <v>1</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
@@ -2703,13 +2567,13 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="M21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="6">
@@ -2717,25 +2581,25 @@
       </c>
       <c r="R21" s="3"/>
       <c r="S21" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
       <c r="AE21" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
@@ -2749,13 +2613,13 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="M22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="6">
@@ -2764,25 +2628,25 @@
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
       <c r="AE22" s="3"/>
       <c r="AF22" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AG22" s="3"/>
     </row>
@@ -2795,13 +2659,13 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="M23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="6">
@@ -2811,25 +2675,25 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AD23" s="3"/>
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.15">
@@ -2841,38 +2705,38 @@
       <c r="G24" s="9"/>
       <c r="H24" s="8"/>
       <c r="M24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="6">
         <v>1</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
@@ -2887,13 +2751,13 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="M25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="6">
@@ -2933,13 +2797,13 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="M26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="6">
@@ -2979,13 +2843,13 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="M27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="6">
@@ -2995,25 +2859,25 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
       <c r="AG27" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.15">
@@ -3025,65 +2889,65 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="M28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="6">
         <v>1</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AA28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AB28" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="AC28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AD28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AE28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AF28" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="AG28" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.15">
@@ -3095,20 +2959,20 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="M29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="6">
         <v>0</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -3135,13 +2999,13 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="M30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="6">
@@ -3149,15 +3013,15 @@
       </c>
       <c r="R30" s="3"/>
       <c r="S30" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
@@ -3179,13 +3043,13 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="M31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="6">
@@ -3194,23 +3058,23 @@
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AB31" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
@@ -3220,13 +3084,13 @@
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.15">
       <c r="M32" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="6">
@@ -3236,47 +3100,47 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AD32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AF32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="AG32" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D8 M12:P27 M29:P30 M32:P32">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:P28">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>M28=M27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:P31">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>M31=M29</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3322,19 +3186,19 @@
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
@@ -3359,11 +3223,11 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.15">
@@ -3398,7 +3262,7 @@
         <v>21</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>10</v>
@@ -3417,32 +3281,32 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.15">
       <c r="L9" s="10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.15">
       <c r="M10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>2</v>
@@ -3486,7 +3350,7 @@
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.15">
       <c r="M11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>3</v>
@@ -3495,19 +3359,19 @@
         <v>9</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q11" s="6">
         <v>0</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -3528,7 +3392,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="M12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>3</v>
@@ -3537,7 +3401,7 @@
         <v>9</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="6">
         <v>1</v>
@@ -3546,13 +3410,13 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
@@ -3570,7 +3434,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="8"/>
       <c r="M13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>3</v>
@@ -3579,7 +3443,7 @@
         <v>9</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q13" s="6">
         <v>2</v>
@@ -3591,13 +3455,13 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
@@ -3612,7 +3476,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="M14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>3</v>
@@ -3621,7 +3485,7 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q14" s="6">
         <v>3</v>
@@ -3636,13 +3500,13 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.15">
@@ -3654,53 +3518,53 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="M15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="6">
         <v>0</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="X15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="AA15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AC15" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.15">
@@ -3712,53 +3576,53 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="M16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="X16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="AA16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB16" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AC16" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.15">
@@ -3770,16 +3634,16 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="M17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q17" s="6">
         <v>0</v>
@@ -3806,37 +3670,37 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="M18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
@@ -3850,38 +3714,38 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="M19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q19" s="6">
         <v>2</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="AC19" s="3"/>
     </row>
@@ -3894,16 +3758,16 @@
       <c r="G20" s="9"/>
       <c r="H20" s="8"/>
       <c r="M20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q20" s="6">
         <v>3</v>
@@ -3911,22 +3775,22 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.15">
@@ -3938,13 +3802,13 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="M21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="6">
@@ -3972,38 +3836,38 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="M22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="6">
         <v>1</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="U22" s="3"/>
       <c r="V22" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
@@ -4018,13 +3882,13 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="M23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="6">
@@ -4034,25 +3898,25 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB23" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.15">
@@ -4064,13 +3928,13 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="M24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="6">
@@ -4098,13 +3962,13 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="M25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="6">
@@ -4114,19 +3978,19 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
       <c r="Y25" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.15">
@@ -4138,50 +4002,50 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="M26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="6">
         <v>10</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W26" s="3"/>
       <c r="X26" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AC26" s="3"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.15">
       <c r="M27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="6">
@@ -4189,32 +4053,32 @@
       </c>
       <c r="R27" s="3"/>
       <c r="S27" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.15">
       <c r="M28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="6">
@@ -4223,7 +4087,7 @@
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -4238,648 +4102,11 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:E7 M11:P28">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="2.125" style="5"/>
-    <col min="3" max="3" width="10.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.125" style="5"/>
-    <col min="12" max="12" width="2.375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="24" width="2.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="2.125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="C10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="L12" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="M13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="4">
-        <v>1</v>
-      </c>
-      <c r="S13" s="4">
-        <v>2</v>
-      </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="M14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>0</v>
-      </c>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="M15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>1</v>
-      </c>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="8"/>
-      <c r="M16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>2</v>
-      </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="M17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>3</v>
-      </c>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="M18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>0</v>
-      </c>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="M19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>1</v>
-      </c>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="M20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>2</v>
-      </c>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="M21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q21" s="6">
-        <v>3</v>
-      </c>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="8"/>
-      <c r="M22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="6">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="M23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="6">
-        <v>1</v>
-      </c>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="M24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="6">
-        <v>2</v>
-      </c>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="M25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="6">
-        <v>3</v>
-      </c>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C4:D10">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>C4=C3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14:P25">
-    <cfRule type="expression" dxfId="8" priority="1">
-      <formula>M14=M13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>